<commit_message>
create Excel if not exists
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMP\OleObject Excel 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMP99\oleobject_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59968808-628F-41F2-8799-A540DE43CEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E37E8F-995A-4BC7-8020-13C2C935DF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{673FD0A7-298B-4299-97A4-E38077A79589}"/>
+    <workbookView xWindow="32370" yWindow="1950" windowWidth="24180" windowHeight="11700" xr2:uid="{673FD0A7-298B-4299-97A4-E38077A79589}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Alfa</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Free</t>
   </si>
   <si>
-    <t>202</t>
-  </si>
-  <si>
     <t>Beta</t>
   </si>
   <si>
@@ -75,6 +72,18 @@
   </si>
   <si>
     <t>IDE</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
   </si>
 </sst>
 </file>
@@ -145,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +194,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -291,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,17 +465,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
-        <v>101</v>
+      <c r="A1" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5">
-        <v>303</v>
-      </c>
-      <c r="D1" s="2">
-        <v>404</v>
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -474,13 +483,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -488,13 +497,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,13 +511,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>